<commit_message>
previo a separar la formula
</commit_message>
<xml_diff>
--- a/wikidata/hal_field_audit_out/Wikidata_upec_chemical_20_rev2.xlsx
+++ b/wikidata/hal_field_audit_out/Wikidata_upec_chemical_20_rev2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanda\Documents\Langara_College\DANA-4850-001-Capstone_Project\hall-api-test-db-mysql\wikidata\hal_field_audit_out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DCA4B8-A2E5-4E53-ABDE-841AFB2973D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA672265-47AC-4F95-AE39-2461CD77BD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B94CFD69-61F1-4950-B09D-9EE9202C93BD}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="322">
   <si>
     <t>docid</t>
   </si>
@@ -147,15 +147,6 @@
     <t>Q137056</t>
   </si>
   <si>
-    <t>11975888z</t>
-  </si>
-  <si>
-    <t>Q3382117</t>
-  </si>
-  <si>
-    <t>chemical phenomenon</t>
-  </si>
-  <si>
     <t>Ni-MH batteries</t>
   </si>
   <si>
@@ -849,18 +840,6 @@
     <t>Q505668</t>
   </si>
   <si>
-    <t>Tem</t>
-  </si>
-  <si>
-    <t>Q36531</t>
-  </si>
-  <si>
-    <t>12167223r</t>
-  </si>
-  <si>
-    <t>Q1288568;Q34770</t>
-  </si>
-  <si>
     <t>chromium</t>
   </si>
   <si>
@@ -987,25 +966,46 @@
     <t>political group of the European Parliament;non-attached</t>
   </si>
   <si>
-    <t>field of study;method</t>
-  </si>
-  <si>
     <t>Mod2b vs 2a</t>
   </si>
   <si>
-    <t>Q110548120</t>
-  </si>
-  <si>
-    <t>Q11060274;Q18218093;Q838948</t>
-  </si>
-  <si>
-    <t>language;modern language</t>
-  </si>
-  <si>
-    <t>funding body;open-access publisher;government agency;vice-ministerial level institution</t>
-  </si>
-  <si>
-    <t>print;work of art;etching print</t>
+    <t>European route E80</t>
+  </si>
+  <si>
+    <t>Q877647</t>
+  </si>
+  <si>
+    <t>Q34442</t>
+  </si>
+  <si>
+    <t>road</t>
+  </si>
+  <si>
+    <t>Q101007233;Q4220917</t>
+  </si>
+  <si>
+    <t>11952827m</t>
+  </si>
+  <si>
+    <t>Q118733587</t>
+  </si>
+  <si>
+    <t>type of meteorological phenomenon</t>
+  </si>
+  <si>
+    <t>boiler feedwater</t>
+  </si>
+  <si>
+    <t>Q351261</t>
+  </si>
+  <si>
+    <t>method;field of study</t>
+  </si>
+  <si>
+    <t>film award;film critics association</t>
+  </si>
+  <si>
+    <t>open-access publisher;funding body;vice-ministerial level institution;government agency</t>
   </si>
 </sst>
 </file>
@@ -1148,7 +1148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1364,6 +1364,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1525,7 +1531,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1533,6 +1539,7 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -8691,14 +8698,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76B0F430-0357-4ED2-80C0-C755800CD5D2}">
   <dimension ref="A1:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="A10:Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.109375" customWidth="1"/>
     <col min="23" max="23" width="11.88671875" customWidth="1"/>
     <col min="24" max="24" width="10.6640625" customWidth="1"/>
@@ -8748,31 +8755,31 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="V1" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>196</v>
-      </c>
       <c r="Y1" s="3" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
@@ -8942,10 +8949,10 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>17</v>
@@ -8954,7 +8961,7 @@
         <v>100</v>
       </c>
       <c r="L4" s="6">
-        <v>137.1</v>
+        <v>68.5</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
@@ -9160,18 +9167,18 @@
         <v>24</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>17</v>
@@ -9180,7 +9187,7 @@
         <v>100</v>
       </c>
       <c r="L7" s="6">
-        <v>144.30000000000001</v>
+        <v>125.5</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
@@ -9209,17 +9216,17 @@
         <v>Q505668</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="V7" s="3" t="str">
         <f t="shared" si="2"/>
         <v>Mod</v>
       </c>
       <c r="W7" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="X7" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="Y7" s="3" t="str">
         <f t="shared" si="3"/>
@@ -9321,10 +9328,10 @@
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>17</v>
@@ -9333,13 +9340,13 @@
         <v>100</v>
       </c>
       <c r="L9" s="6">
-        <v>222.4</v>
+        <v>85.9</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="O9" s="1" t="str">
         <f>VLOOKUP(C9,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -9395,20 +9402,18 @@
         <v>32</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>317</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>17</v>
@@ -9417,14 +9422,10 @@
         <v>100</v>
       </c>
       <c r="L10" s="6">
-        <v>165</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>37</v>
-      </c>
+        <v>122.7</v>
+      </c>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
       <c r="O10" s="1" t="str">
         <f>VLOOKUP(C10,[1]Sheet2!$C:$N,3,FALSE)</f>
         <v>Q5173028</v>
@@ -9447,14 +9448,14 @@
       </c>
       <c r="T10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Q137056</v>
+        <v>Q351261</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="V10" s="3" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Mod</v>
       </c>
       <c r="W10" t="s">
         <v>33</v>
@@ -9464,7 +9465,7 @@
       </c>
       <c r="Y10" s="3" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Mod</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
@@ -9475,7 +9476,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -9549,7 +9550,7 @@
         <v>31</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -9623,23 +9624,21 @@
         <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>269</v>
+        <v>309</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>271</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>17</v>
@@ -9648,13 +9647,13 @@
         <v>100</v>
       </c>
       <c r="L13" s="6">
-        <v>120.3</v>
+        <v>115.8</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>272</v>
+        <v>311</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="O13" s="1" t="str">
         <f>VLOOKUP(C13,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -9678,20 +9677,20 @@
       </c>
       <c r="T13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Q36531</v>
+        <v>Q877647</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="V13" s="5" t="str">
         <f t="shared" si="2"/>
         <v>Mod</v>
       </c>
       <c r="W13" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="X13" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="Y13" s="3" t="str">
         <f t="shared" si="3"/>
@@ -9706,7 +9705,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -9777,7 +9776,7 @@
         <v>1060481</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="6">
         <v>20902069</v>
@@ -9851,24 +9850,24 @@
         <v>1060481</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>45</v>
+        <v>196</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>46</v>
+        <v>197</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>17</v>
@@ -9877,10 +9876,10 @@
         <v>100</v>
       </c>
       <c r="L16" s="6">
-        <v>61</v>
+        <v>113.2</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>47</v>
+        <v>313</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>320</v>
@@ -9907,7 +9906,7 @@
       </c>
       <c r="T16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Q4501917</v>
+        <v>Q1206671</v>
       </c>
       <c r="U16" s="3" t="str">
         <f t="shared" si="1"/>
@@ -9917,11 +9916,11 @@
         <f t="shared" si="2"/>
         <v>Mod</v>
       </c>
-      <c r="W16" t="s">
-        <v>199</v>
-      </c>
-      <c r="X16" t="s">
-        <v>200</v>
+      <c r="W16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="Y16" s="3" t="str">
         <f t="shared" si="3"/>
@@ -9933,24 +9932,24 @@
         <v>1060481</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="E17" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>17</v>
@@ -9959,13 +9958,13 @@
         <v>100</v>
       </c>
       <c r="L17" s="6">
-        <v>79.8</v>
+        <v>63.3</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="O17" s="1" t="str">
         <f>VLOOKUP(C17,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -10000,10 +9999,10 @@
         <v/>
       </c>
       <c r="W17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="X17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Y17" s="3" t="str">
         <f t="shared" si="3"/>
@@ -10015,7 +10014,7 @@
         <v>1060481</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" s="6">
         <v>21074094</v>
@@ -10089,7 +10088,7 @@
         <v>1060481</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C19" s="6">
         <v>51173134</v>
@@ -10163,10 +10162,10 @@
         <v>1064801</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -10237,10 +10236,10 @@
         <v>1064801</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -10311,10 +10310,10 @@
         <v>1064801</v>
       </c>
       <c r="B22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -10385,16 +10384,16 @@
         <v>1064801</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -10411,13 +10410,13 @@
         <v>96.8</v>
       </c>
       <c r="L23" s="6">
-        <v>141.9</v>
+        <v>81.099999999999994</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O23" s="1" t="str">
         <f>VLOOKUP(C23,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -10452,10 +10451,10 @@
         <v/>
       </c>
       <c r="W23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="X23" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Y23" s="3" t="str">
         <f t="shared" si="3"/>
@@ -10467,10 +10466,10 @@
         <v>1067996</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -10541,24 +10540,26 @@
         <v>1067996</v>
       </c>
       <c r="B25" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>59</v>
-      </c>
       <c r="E25" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="F25" s="6"/>
+        <v>58</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>314</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>266</v>
+        <v>21</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>17</v>
@@ -10567,13 +10568,13 @@
         <v>100</v>
       </c>
       <c r="L25" s="6">
-        <v>75.599999999999994</v>
+        <v>151.80000000000001</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N25" s="6" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="O25" s="1" t="str">
         <f>VLOOKUP(C25,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -10597,7 +10598,7 @@
       </c>
       <c r="T25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>Q110548120</v>
+        <v>Q8074</v>
       </c>
       <c r="U25" s="3" t="str">
         <f t="shared" si="1"/>
@@ -10605,17 +10606,17 @@
       </c>
       <c r="V25" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>Mod</v>
+        <v/>
       </c>
       <c r="W25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="X25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Y25" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>Mod</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
@@ -10623,10 +10624,10 @@
         <v>1067996</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -10697,10 +10698,10 @@
         <v>1067996</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -10771,10 +10772,10 @@
         <v>1067996</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -10845,10 +10846,10 @@
         <v>1078652</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H29" t="s">
         <v>16</v>
@@ -10913,22 +10914,22 @@
         <v>1078652</v>
       </c>
       <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
         <v>65</v>
       </c>
-      <c r="C30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" t="s">
-        <v>68</v>
-      </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H30" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I30" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J30" t="s">
         <v>17</v>
@@ -10972,10 +10973,10 @@
         <v/>
       </c>
       <c r="W30" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="X30" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="Y30" s="3" t="str">
         <f t="shared" si="3"/>
@@ -10987,22 +10988,22 @@
         <v>1078652</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I31" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J31" t="s">
         <v>17</v>
@@ -11046,10 +11047,10 @@
         <v>Mod</v>
       </c>
       <c r="W31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="X31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="Y31" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11061,10 +11062,10 @@
         <v>1078652</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H32" t="s">
         <v>16</v>
@@ -11129,10 +11130,10 @@
         <v>1078652</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H33" t="s">
         <v>16</v>
@@ -11197,16 +11198,16 @@
         <v>1078652</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H34" t="s">
         <v>21</v>
@@ -11256,10 +11257,10 @@
         <v/>
       </c>
       <c r="W34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="X34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Y34" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11271,16 +11272,16 @@
         <v>1078652</v>
       </c>
       <c r="B35" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H35" t="s">
         <v>21</v>
@@ -11298,10 +11299,10 @@
         <v>147.9</v>
       </c>
       <c r="M35" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="N35" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="O35" s="1" t="str">
         <f>VLOOKUP(C35,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -11336,10 +11337,10 @@
         <v>Mod</v>
       </c>
       <c r="W35" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="X35" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="Y35" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11351,10 +11352,10 @@
         <v>1078896</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H36" t="s">
         <v>16</v>
@@ -11419,16 +11420,16 @@
         <v>1078896</v>
       </c>
       <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
         <v>77</v>
       </c>
-      <c r="C37" t="s">
-        <v>79</v>
-      </c>
-      <c r="D37" t="s">
-        <v>80</v>
-      </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H37" t="s">
         <v>21</v>
@@ -11446,10 +11447,10 @@
         <v>216.3</v>
       </c>
       <c r="M37" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="N37" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O37" s="1" t="str">
         <f>VLOOKUP(C37,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -11484,10 +11485,10 @@
         <v/>
       </c>
       <c r="W37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="X37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="Y37" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11499,16 +11500,16 @@
         <v>1078896</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E38" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="H38" t="s">
         <v>21</v>
@@ -11526,10 +11527,10 @@
         <v>86.5</v>
       </c>
       <c r="M38" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N38" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="O38" s="1">
         <f>VLOOKUP(C38,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -11564,10 +11565,10 @@
         <v>Mod</v>
       </c>
       <c r="W38" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="X38" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="Y38" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11579,10 +11580,10 @@
         <v>1083001</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H39" t="s">
         <v>16</v>
@@ -11647,10 +11648,10 @@
         <v>1083001</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H40" t="s">
         <v>16</v>
@@ -11715,22 +11716,22 @@
         <v>1083001</v>
       </c>
       <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
         <v>85</v>
       </c>
-      <c r="C41" t="s">
-        <v>88</v>
-      </c>
       <c r="D41" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="E41" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="H41" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I41" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J41" t="s">
         <v>17</v>
@@ -11742,10 +11743,10 @@
         <v>90.8</v>
       </c>
       <c r="M41" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="N41" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="O41" s="1" t="str">
         <f>VLOOKUP(C41,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -11780,10 +11781,10 @@
         <v>Mod</v>
       </c>
       <c r="W41" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="X41" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="Y41" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11795,16 +11796,16 @@
         <v>1083001</v>
       </c>
       <c r="B42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D42" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H42" t="s">
         <v>21</v>
@@ -11854,10 +11855,10 @@
         <v>Mod</v>
       </c>
       <c r="W42" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="X42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="Y42" s="3" t="str">
         <f t="shared" si="3"/>
@@ -11869,10 +11870,10 @@
         <v>1083004</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H43" t="s">
         <v>16</v>
@@ -11937,22 +11938,22 @@
         <v>1083004</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D44" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E44" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H44" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I44" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J44" t="s">
         <v>17</v>
@@ -11964,10 +11965,10 @@
         <v>198</v>
       </c>
       <c r="M44" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="N44" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="O44" s="1" t="str">
         <f>VLOOKUP(C44,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12002,10 +12003,10 @@
         <v>Mod</v>
       </c>
       <c r="W44" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="X44" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="Y44" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12017,22 +12018,22 @@
         <v>1083004</v>
       </c>
       <c r="B45" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" t="s">
         <v>90</v>
       </c>
-      <c r="C45" t="s">
-        <v>93</v>
-      </c>
       <c r="D45" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E45" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H45" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I45" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J45" t="s">
         <v>17</v>
@@ -12076,10 +12077,10 @@
         <v>Mod</v>
       </c>
       <c r="W45" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="X45" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="Y45" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12091,10 +12092,10 @@
         <v>1083007</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H46" t="s">
         <v>16</v>
@@ -12159,22 +12160,22 @@
         <v>1083007</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C47" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H47" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I47" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J47" t="s">
         <v>17</v>
@@ -12186,10 +12187,10 @@
         <v>171.9</v>
       </c>
       <c r="M47" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="N47" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O47" s="1" t="str">
         <f>VLOOKUP(C47,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12224,10 +12225,10 @@
         <v/>
       </c>
       <c r="W47" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="X47" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Y47" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12239,22 +12240,22 @@
         <v>1083007</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E48" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H48" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I48" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J48" t="s">
         <v>17</v>
@@ -12266,10 +12267,10 @@
         <v>86.9</v>
       </c>
       <c r="M48" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N48" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O48" s="1" t="str">
         <f>VLOOKUP(C48,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12304,10 +12305,10 @@
         <v>Mod</v>
       </c>
       <c r="W48" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="X48" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="Y48" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12319,22 +12320,22 @@
         <v>1083007</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C49" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="E49" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H49" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I49" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J49" t="s">
         <v>17</v>
@@ -12346,10 +12347,10 @@
         <v>105.9</v>
       </c>
       <c r="M49" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N49" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O49" s="1" t="str">
         <f>VLOOKUP(C49,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12384,10 +12385,10 @@
         <v>Mod</v>
       </c>
       <c r="W49" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="X49" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="Y49" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12399,10 +12400,10 @@
         <v>1083014</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H50" t="s">
         <v>16</v>
@@ -12467,22 +12468,22 @@
         <v>1083014</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D51" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E51" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="H51" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I51" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J51" t="s">
         <v>17</v>
@@ -12494,10 +12495,10 @@
         <v>102.1</v>
       </c>
       <c r="M51" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N51" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O51" s="1" t="str">
         <f>VLOOKUP(C51,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12532,10 +12533,10 @@
         <v>Mod</v>
       </c>
       <c r="W51" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="X51" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="Y51" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12547,22 +12548,22 @@
         <v>1083014</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D52" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E52" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H52" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I52" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J52" t="s">
         <v>17</v>
@@ -12574,10 +12575,10 @@
         <v>101</v>
       </c>
       <c r="M52" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="N52" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="O52" s="1" t="str">
         <f>VLOOKUP(C52,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12612,10 +12613,10 @@
         <v>Mod</v>
       </c>
       <c r="W52" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="X52" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="Y52" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12627,22 +12628,22 @@
         <v>1083157</v>
       </c>
       <c r="B53" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D53" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E53" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H53" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I53" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J53" t="s">
         <v>17</v>
@@ -12654,10 +12655,10 @@
         <v>171.3</v>
       </c>
       <c r="M53" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="N53" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="O53" s="1">
         <f>VLOOKUP(C53,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -12692,10 +12693,10 @@
         <v>Mod</v>
       </c>
       <c r="W53" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="X53" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="Y53" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12707,10 +12708,10 @@
         <v>1083157</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H54" t="s">
         <v>16</v>
@@ -12775,10 +12776,10 @@
         <v>1083160</v>
       </c>
       <c r="B55" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H55" t="s">
         <v>16</v>
@@ -12843,10 +12844,10 @@
         <v>1083160</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C56" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H56" t="s">
         <v>16</v>
@@ -12911,22 +12912,22 @@
         <v>1084520</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D57" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E57" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H57" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I57" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J57" t="s">
         <v>17</v>
@@ -12970,10 +12971,10 @@
         <v>Mod</v>
       </c>
       <c r="W57" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="X57" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="Y57" s="3" t="str">
         <f t="shared" si="3"/>
@@ -12985,22 +12986,22 @@
         <v>1084520</v>
       </c>
       <c r="B58" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" t="s">
         <v>108</v>
       </c>
-      <c r="C58" t="s">
-        <v>110</v>
-      </c>
-      <c r="D58" t="s">
-        <v>111</v>
-      </c>
       <c r="E58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H58" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I58" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J58" t="s">
         <v>17</v>
@@ -13044,10 +13045,10 @@
         <v/>
       </c>
       <c r="W58" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="X58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y58" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13059,22 +13060,22 @@
         <v>1084520</v>
       </c>
       <c r="B59" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D59" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E59" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="H59" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I59" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J59" t="s">
         <v>17</v>
@@ -13118,10 +13119,10 @@
         <v>Mod</v>
       </c>
       <c r="W59" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="X59" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="Y59" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13133,22 +13134,22 @@
         <v>1084520</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D60" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E60" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="H60" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I60" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J60" t="s">
         <v>17</v>
@@ -13160,10 +13161,10 @@
         <v>154.6</v>
       </c>
       <c r="M60" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N60" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O60" s="1" t="str">
         <f>VLOOKUP(C60,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -13198,10 +13199,10 @@
         <v>Mod</v>
       </c>
       <c r="W60" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="X60" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="Y60" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13213,22 +13214,22 @@
         <v>1084520</v>
       </c>
       <c r="B61" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D61" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E61" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H61" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I61" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J61" t="s">
         <v>17</v>
@@ -13272,10 +13273,10 @@
         <v/>
       </c>
       <c r="W61" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="X61" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Y61" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13287,22 +13288,22 @@
         <v>1084520</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D62" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E62" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H62" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I62" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J62" t="s">
         <v>17</v>
@@ -13346,10 +13347,10 @@
         <v>Mod</v>
       </c>
       <c r="W62" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="X62" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="Y62" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13361,22 +13362,22 @@
         <v>1084657</v>
       </c>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C63" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D63" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E63" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="H63" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I63" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J63" t="s">
         <v>17</v>
@@ -13388,10 +13389,10 @@
         <v>149.5</v>
       </c>
       <c r="M63" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="N63" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O63" s="1" t="str">
         <f>VLOOKUP(C63,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -13426,10 +13427,10 @@
         <v>Mod</v>
       </c>
       <c r="W63" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="X63" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="Y63" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13441,25 +13442,25 @@
         <v>1084657</v>
       </c>
       <c r="B64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C64" t="s">
+        <v>118</v>
+      </c>
+      <c r="D64" t="s">
         <v>119</v>
       </c>
-      <c r="C64" t="s">
+      <c r="E64" t="s">
+        <v>120</v>
+      </c>
+      <c r="F64" t="s">
         <v>121</v>
       </c>
-      <c r="D64" t="s">
-        <v>122</v>
-      </c>
-      <c r="E64" t="s">
-        <v>123</v>
-      </c>
-      <c r="F64" t="s">
-        <v>124</v>
-      </c>
       <c r="H64" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I64" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J64" t="s">
         <v>17</v>
@@ -13471,10 +13472,10 @@
         <v>159</v>
       </c>
       <c r="M64" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O64" s="1" t="str">
         <f>VLOOKUP(C64,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -13509,10 +13510,10 @@
         <v/>
       </c>
       <c r="W64" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="X64" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="Y64" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13524,25 +13525,25 @@
         <v>1084657</v>
       </c>
       <c r="B65" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F65">
         <v>119510333</v>
       </c>
       <c r="H65" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I65" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J65" t="s">
         <v>17</v>
@@ -13554,10 +13555,10 @@
         <v>219.6</v>
       </c>
       <c r="M65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N65" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O65" s="1" t="str">
         <f>VLOOKUP(C65,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -13592,10 +13593,10 @@
         <v/>
       </c>
       <c r="W65" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="X65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Y65" s="3" t="str">
         <f t="shared" si="3"/>
@@ -13607,10 +13608,10 @@
         <v>1084657</v>
       </c>
       <c r="B66" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C66" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H66" t="s">
         <v>16</v>
@@ -13675,22 +13676,22 @@
         <v>1084657</v>
       </c>
       <c r="B67" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D67" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E67" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="H67" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I67" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J67" t="s">
         <v>17</v>
@@ -13702,10 +13703,10 @@
         <v>118.4</v>
       </c>
       <c r="M67" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N67" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="O67" s="1" t="str">
         <f>VLOOKUP(C67,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -13740,10 +13741,10 @@
         <v>Mod</v>
       </c>
       <c r="W67" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="X67" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="Y67" s="3" t="str">
         <f t="shared" ref="Y67:Y104" si="6">IF(X67&lt;&gt;E67,"Mod","")</f>
@@ -13755,10 +13756,10 @@
         <v>1084678</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H68" t="s">
         <v>16</v>
@@ -13804,7 +13805,7 @@
         <v>ok</v>
       </c>
       <c r="V68" s="3" t="str">
-        <f t="shared" ref="V67:V104" si="7">IF(T68&lt;&gt;Q68,"Mod","")</f>
+        <f t="shared" ref="V68:V104" si="7">IF(T68&lt;&gt;Q68,"Mod","")</f>
         <v/>
       </c>
       <c r="W68">
@@ -13823,22 +13824,22 @@
         <v>1084678</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D69" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E69" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H69" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I69" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J69" t="s">
         <v>17</v>
@@ -13882,10 +13883,10 @@
         <v>Mod</v>
       </c>
       <c r="W69" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="X69" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="Y69" s="3" t="str">
         <f t="shared" si="6"/>
@@ -13897,10 +13898,10 @@
         <v>1084678</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H70" t="s">
         <v>16</v>
@@ -13965,10 +13966,10 @@
         <v>1084678</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C71" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H71" t="s">
         <v>16</v>
@@ -14033,22 +14034,22 @@
         <v>1084678</v>
       </c>
       <c r="B72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" t="s">
         <v>134</v>
       </c>
-      <c r="C72" t="s">
-        <v>137</v>
-      </c>
       <c r="D72" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E72" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H72" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I72" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J72" t="s">
         <v>17</v>
@@ -14060,10 +14061,10 @@
         <v>180.4</v>
       </c>
       <c r="M72" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="N72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="O72" s="1" t="str">
         <f>VLOOKUP(C72,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14098,10 +14099,10 @@
         <v/>
       </c>
       <c r="W72" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="X72" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="Y72" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14113,16 +14114,16 @@
         <v>1084678</v>
       </c>
       <c r="B73" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C73" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H73" t="s">
         <v>21</v>
@@ -14172,10 +14173,10 @@
         <v/>
       </c>
       <c r="W73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="X73" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="Y73" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14187,25 +14188,25 @@
         <v>1086746</v>
       </c>
       <c r="B74" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C74" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D74" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E74" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F74" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H74" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I74" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J74" t="s">
         <v>17</v>
@@ -14217,10 +14218,10 @@
         <v>144.1</v>
       </c>
       <c r="M74" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="N74" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="O74" s="1">
         <f>VLOOKUP(C74,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14255,10 +14256,10 @@
         <v>Mod</v>
       </c>
       <c r="W74" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="X74" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="Y74" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14270,25 +14271,25 @@
         <v>1086746</v>
       </c>
       <c r="B75" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C75" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D75" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E75" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F75">
         <v>119470591</v>
       </c>
       <c r="H75" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I75" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J75" t="s">
         <v>17</v>
@@ -14300,10 +14301,10 @@
         <v>149.80000000000001</v>
       </c>
       <c r="M75" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="N75" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="O75" s="1">
         <f>VLOOKUP(C75,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14338,10 +14339,10 @@
         <v>Mod</v>
       </c>
       <c r="W75" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="X75" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="Y75" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14353,25 +14354,25 @@
         <v>1086746</v>
       </c>
       <c r="B76" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" t="s">
         <v>145</v>
       </c>
-      <c r="C76" t="s">
-        <v>148</v>
-      </c>
       <c r="D76" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E76" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F76" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H76" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I76" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J76" t="s">
         <v>17</v>
@@ -14383,10 +14384,10 @@
         <v>163.80000000000001</v>
       </c>
       <c r="M76" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="N76" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O76" s="1">
         <f>VLOOKUP(C76,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14421,10 +14422,10 @@
         <v>Mod</v>
       </c>
       <c r="W76" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="X76" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="Y76" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14436,25 +14437,25 @@
         <v>1086746</v>
       </c>
       <c r="B77" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D77" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E77" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F77">
         <v>118650631</v>
       </c>
       <c r="H77" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I77" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J77" t="s">
         <v>17</v>
@@ -14466,10 +14467,10 @@
         <v>151.5</v>
       </c>
       <c r="M77" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N77" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="O77" s="1">
         <f>VLOOKUP(C77,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14504,10 +14505,10 @@
         <v>Mod</v>
       </c>
       <c r="W77" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="X77" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="Y77" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14519,25 +14520,25 @@
         <v>1086746</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C78" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D78" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E78" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F78" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="H78" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I78" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J78" t="s">
         <v>17</v>
@@ -14549,10 +14550,10 @@
         <v>146.5</v>
       </c>
       <c r="M78" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N78" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="O78" s="1">
         <f>VLOOKUP(C78,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14587,10 +14588,10 @@
         <v>Mod</v>
       </c>
       <c r="W78" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="X78" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="Y78" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14602,25 +14603,25 @@
         <v>1086746</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C79" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D79" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E79" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F79">
         <v>119567697</v>
       </c>
       <c r="H79" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I79" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J79" t="s">
         <v>17</v>
@@ -14632,10 +14633,10 @@
         <v>157.1</v>
       </c>
       <c r="M79" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N79" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="O79" s="1">
         <f>VLOOKUP(C79,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14670,10 +14671,10 @@
         <v>Mod</v>
       </c>
       <c r="W79" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="X79" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Y79" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14685,22 +14686,22 @@
         <v>1086746</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C80" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D80" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E80" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="H80" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I80" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J80" t="s">
         <v>17</v>
@@ -14744,10 +14745,10 @@
         <v>Mod</v>
       </c>
       <c r="W80" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="X80" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="Y80" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14759,22 +14760,22 @@
         <v>1086746</v>
       </c>
       <c r="B81" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C81" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D81" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="E81" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="H81" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I81" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J81" t="s">
         <v>17</v>
@@ -14818,10 +14819,10 @@
         <v>Mod</v>
       </c>
       <c r="W81" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="X81" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="Y81" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14833,22 +14834,22 @@
         <v>1086746</v>
       </c>
       <c r="B82" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C82" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D82" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E82" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="H82" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I82" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J82" t="s">
         <v>17</v>
@@ -14860,10 +14861,10 @@
         <v>148.69999999999999</v>
       </c>
       <c r="M82" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="N82" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="O82" s="1" t="str">
         <f>VLOOKUP(C82,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14898,10 +14899,10 @@
         <v>Mod</v>
       </c>
       <c r="W82" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="X82" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="Y82" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14913,25 +14914,25 @@
         <v>1086746</v>
       </c>
       <c r="B83" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C83" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D83" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="E83" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="F83" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="H83" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I83" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J83" t="s">
         <v>17</v>
@@ -14943,10 +14944,10 @@
         <v>129.6</v>
       </c>
       <c r="M83" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="N83" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="O83" s="1" t="str">
         <f>VLOOKUP(C83,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -14981,10 +14982,10 @@
         <v>Mod</v>
       </c>
       <c r="W83" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="X83" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="Y83" s="3" t="str">
         <f t="shared" si="6"/>
@@ -14996,22 +14997,22 @@
         <v>1086746</v>
       </c>
       <c r="B84" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C84" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D84" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E84" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="H84" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I84" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J84" t="s">
         <v>17</v>
@@ -15023,10 +15024,10 @@
         <v>119.3</v>
       </c>
       <c r="M84" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="N84" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="O84" s="1" t="str">
         <f>VLOOKUP(C84,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -15061,10 +15062,10 @@
         <v>Mod</v>
       </c>
       <c r="W84" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="X84" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="Y84" s="3" t="str">
         <f t="shared" si="6"/>
@@ -15076,10 +15077,10 @@
         <v>1086752</v>
       </c>
       <c r="B85" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C85" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H85" t="s">
         <v>16</v>
@@ -15144,10 +15145,10 @@
         <v>1086752</v>
       </c>
       <c r="B86" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C86" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="H86" t="s">
         <v>16</v>
@@ -15212,10 +15213,10 @@
         <v>1086752</v>
       </c>
       <c r="B87" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" t="s">
         <v>158</v>
-      </c>
-      <c r="C87" t="s">
-        <v>161</v>
       </c>
       <c r="H87" t="s">
         <v>16</v>
@@ -15280,22 +15281,22 @@
         <v>1086752</v>
       </c>
       <c r="B88" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C88" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D88" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E88" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H88" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I88" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J88" t="s">
         <v>17</v>
@@ -15339,10 +15340,10 @@
         <v>Mod</v>
       </c>
       <c r="W88" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="X88" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Y88" s="3" t="str">
         <f t="shared" si="6"/>
@@ -15354,10 +15355,10 @@
         <v>1087358</v>
       </c>
       <c r="B89" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H89" t="s">
         <v>16</v>
@@ -15422,22 +15423,22 @@
         <v>1087358</v>
       </c>
       <c r="B90" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C90" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D90" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E90" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H90" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I90" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J90" t="s">
         <v>17</v>
@@ -15481,10 +15482,10 @@
         <v>Mod</v>
       </c>
       <c r="W90" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="X90" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="Y90" s="3" t="str">
         <f t="shared" si="6"/>
@@ -15496,10 +15497,10 @@
         <v>1087358</v>
       </c>
       <c r="B91" t="s">
+        <v>160</v>
+      </c>
+      <c r="C91" t="s">
         <v>163</v>
-      </c>
-      <c r="C91" t="s">
-        <v>166</v>
       </c>
       <c r="H91" t="s">
         <v>16</v>
@@ -15564,10 +15565,10 @@
         <v>1087358</v>
       </c>
       <c r="B92" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C92" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H92" t="s">
         <v>16</v>
@@ -15632,22 +15633,22 @@
         <v>1087358</v>
       </c>
       <c r="B93" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C93" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D93" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E93" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H93" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I93" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J93" t="s">
         <v>17</v>
@@ -15659,10 +15660,10 @@
         <v>137.30000000000001</v>
       </c>
       <c r="M93" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N93" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O93" s="1" t="str">
         <f>VLOOKUP(C93,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -15697,10 +15698,10 @@
         <v>Mod</v>
       </c>
       <c r="W93" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="X93" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Y93" s="3" t="str">
         <f t="shared" si="6"/>
@@ -15712,22 +15713,22 @@
         <v>1087358</v>
       </c>
       <c r="B94" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C94" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D94" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="E94" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H94" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I94" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J94" t="s">
         <v>17</v>
@@ -15739,10 +15740,10 @@
         <v>113.7</v>
       </c>
       <c r="M94" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="N94" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O94" s="1">
         <f>VLOOKUP(C94,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -15777,10 +15778,10 @@
         <v>Mod</v>
       </c>
       <c r="W94" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="X94" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="Y94" s="3" t="str">
         <f t="shared" si="6"/>
@@ -15792,10 +15793,10 @@
         <v>1088019</v>
       </c>
       <c r="B95" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C95" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H95" t="s">
         <v>16</v>
@@ -15860,10 +15861,10 @@
         <v>1088019</v>
       </c>
       <c r="B96" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C96" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="H96" t="s">
         <v>16</v>
@@ -15928,19 +15929,19 @@
         <v>1088019</v>
       </c>
       <c r="B97" t="s">
+        <v>167</v>
+      </c>
+      <c r="C97" t="s">
         <v>170</v>
       </c>
-      <c r="C97" t="s">
-        <v>173</v>
-      </c>
       <c r="D97" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E97" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F97" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H97" t="s">
         <v>21</v>
@@ -15990,10 +15991,10 @@
         <v>Mod</v>
       </c>
       <c r="W97" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="X97" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="Y97" s="3" t="str">
         <f t="shared" si="6"/>
@@ -16005,10 +16006,10 @@
         <v>1088019</v>
       </c>
       <c r="B98" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C98" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H98" t="s">
         <v>16</v>
@@ -16073,22 +16074,22 @@
         <v>1088019</v>
       </c>
       <c r="B99" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C99" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D99" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E99" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H99" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I99" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J99" t="s">
         <v>17</v>
@@ -16132,10 +16133,10 @@
         <v/>
       </c>
       <c r="W99" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="X99" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Y99" s="3" t="str">
         <f t="shared" si="6"/>
@@ -16147,25 +16148,25 @@
         <v>1088019</v>
       </c>
       <c r="B100" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C100" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D100" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E100" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F100">
         <v>119328276</v>
       </c>
       <c r="H100" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I100" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J100" t="s">
         <v>17</v>
@@ -16177,10 +16178,10 @@
         <v>124.7</v>
       </c>
       <c r="M100" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="N100" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="O100" s="1" t="str">
         <f>VLOOKUP(C100,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -16215,10 +16216,10 @@
         <v/>
       </c>
       <c r="W100" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="X100" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Y100" s="3" t="str">
         <f t="shared" si="6"/>
@@ -16230,16 +16231,16 @@
         <v>1088019</v>
       </c>
       <c r="B101" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C101" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D101" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E101" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H101" t="s">
         <v>21</v>
@@ -16289,10 +16290,10 @@
         <v>Mod</v>
       </c>
       <c r="W101" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="X101" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="Y101" s="3" t="str">
         <f t="shared" si="6"/>
@@ -16304,19 +16305,19 @@
         <v>1088019</v>
       </c>
       <c r="B102" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C102" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D102" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E102" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F102" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H102" t="s">
         <v>21</v>
@@ -16334,10 +16335,10 @@
         <v>102.6</v>
       </c>
       <c r="M102" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="N102" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="O102" s="1" t="str">
         <f>VLOOKUP(C102,[1]Sheet2!$C:$N,3,FALSE)</f>
@@ -16372,10 +16373,10 @@
         <v>Mod</v>
       </c>
       <c r="W102" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="X102" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="Y102" s="3" t="str">
         <f t="shared" si="6"/>
@@ -16387,25 +16388,25 @@
         <v>1088019</v>
       </c>
       <c r="B103" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C103" t="s">
+        <v>182</v>
+      </c>
+      <c r="D103" t="s">
+        <v>183</v>
+      </c>
+      <c r="E103" t="s">
+        <v>184</v>
+      </c>
+      <c r="F103" t="s">
         <v>185</v>
       </c>
-      <c r="D103" t="s">
-        <v>186</v>
-      </c>
-      <c r="E103" t="s">
-        <v>187</v>
-      </c>
-      <c r="F103" t="s">
-        <v>188</v>
-      </c>
       <c r="H103" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I103" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J103" t="s">
         <v>17</v>
@@ -16449,10 +16450,10 @@
         <v/>
       </c>
       <c r="W103" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="X103" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Y103" s="3" t="str">
         <f t="shared" si="6"/>
@@ -16464,25 +16465,25 @@
         <v>1088019</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C104" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D104" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E104" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F104">
         <v>119788740</v>
       </c>
       <c r="H104" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="I104" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J104" t="s">
         <v>17</v>
@@ -16526,10 +16527,10 @@
         <v/>
       </c>
       <c r="W104" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="X104" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Y104" s="3" t="str">
         <f t="shared" si="6"/>

</xml_diff>